<commit_message>
Added tooltips and action pulsing animation. Truncated attack sounds and removed Pulse spawn sound to reduce overall noise.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
   <si>
     <t>Event Name</t>
   </si>
@@ -37,37 +37,40 @@
     <t>Pulse Spawn</t>
   </si>
   <si>
+    <t>Disabled (see notes)</t>
+  </si>
+  <si>
+    <t>Sound Effect</t>
+  </si>
+  <si>
+    <t>Short synth note when a new pulse appears in the bottom left of the screen.</t>
+  </si>
+  <si>
+    <t>Synth note</t>
+  </si>
+  <si>
+    <t>Removed to reduce audio clutter.</t>
+  </si>
+  <si>
+    <t>Created using synths in Reaper</t>
+  </si>
+  <si>
+    <t>Source Block Receives Energy</t>
+  </si>
+  <si>
+    <t>Dropped (see notes)</t>
+  </si>
+  <si>
+    <t>Higher pitched synth note when a source block takes in energy from a passing pulse.</t>
+  </si>
+  <si>
+    <t>I felt that this sound would occur too frequently, drowning out more important sounds.</t>
+  </si>
+  <si>
+    <t>Place Block</t>
+  </si>
+  <si>
     <t>Events Implemented</t>
-  </si>
-  <si>
-    <t>Sound Effect</t>
-  </si>
-  <si>
-    <t>Short synth note when a new pulse appears in the bottom left of the screen.</t>
-  </si>
-  <si>
-    <t>Synth note</t>
-  </si>
-  <si>
-    <t>Created inside the music track to prevent the two from desyncing.</t>
-  </si>
-  <si>
-    <t>Created using synths in Reaper</t>
-  </si>
-  <si>
-    <t>Source Block Receives Energy</t>
-  </si>
-  <si>
-    <t>Dropped</t>
-  </si>
-  <si>
-    <t>Higher pitched synth note when a source block takes in energy from a passing pulse.</t>
-  </si>
-  <si>
-    <t>I felt that this sound would occur too frequently, cluttering the game's audio.</t>
-  </si>
-  <si>
-    <t>Place Block</t>
   </si>
   <si>
     <t>Interface</t>
@@ -197,6 +200,9 @@
     <t>Fire crackling sound</t>
   </si>
   <si>
+    <t>Truncated to reduce audio clutter.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <color rgb="FF1155CC"/>
@@ -220,18 +226,12 @@
     <t>Attack - Electric</t>
   </si>
   <si>
-    <t>Events Implemented*</t>
-  </si>
-  <si>
     <t>Sparking when player attacks with Electric element.</t>
   </si>
   <si>
     <t>Elecricity sound</t>
   </si>
   <si>
-    <t>Without electric blocks available, this sound cannot be played. This will be fixed for the next miestone.</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <color rgb="FF1155CC"/>
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>Ice / glass shattering sound</t>
-  </si>
-  <si>
-    <t>Without ice blocks available, this sound cannot be played. This will be fixed for the next miestone.</t>
   </si>
   <si>
     <r>
@@ -448,9 +445,6 @@
     <t>Battle Music Intro</t>
   </si>
   <si>
-    <t>Created in Reaper</t>
-  </si>
-  <si>
     <t>Music</t>
   </si>
   <si>
@@ -460,7 +454,7 @@
     <t>Synths</t>
   </si>
   <si>
-    <t>Still working on refactoring code to allow for time to play this intro before pulses begin generating.</t>
+    <t>Added at the start of Battle Music event in FMOD.</t>
   </si>
   <si>
     <r>
@@ -560,7 +554,7 @@
       <color rgb="FF0000FF"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -575,26 +569,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
-        <bgColor rgb="FFB6D7A8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFE06666"/>
         <bgColor rgb="FFE06666"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA4C2F4"/>
-        <bgColor rgb="FFA4C2F4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD966"/>
-        <bgColor rgb="FFFFD966"/>
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
   </fills>
@@ -624,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -658,10 +640,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
@@ -674,16 +653,12 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -959,7 +934,7 @@
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -979,482 +954,486 @@
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>8</v>
+      <c r="B4" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14" t="s">
         <v>22</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14" t="s">
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
+      <c r="A7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="16" t="s">
         <v>33</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="14" t="s">
         <v>37</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="15" t="s">
         <v>40</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14" t="s">
-        <v>41</v>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>8</v>
+        <v>43</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>43</v>
+      <c r="D11" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="13"/>
+        <v>45</v>
+      </c>
+      <c r="F11" s="12"/>
       <c r="G11" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>8</v>
+      <c r="A12" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="13"/>
+        <v>49</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="G12" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>51</v>
+      <c r="A13" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>51</v>
+      <c r="B14" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="17" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="14" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>8</v>
+      <c r="B15" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="17" t="s">
+    </row>
+    <row r="16">
+      <c r="A16" s="14" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="15" t="s">
+      <c r="B16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="D16" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="15" t="s">
+      <c r="C17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="F17" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="9" t="s">
+    </row>
+    <row r="18">
+      <c r="A18" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="6" t="s">
+    </row>
+    <row r="19">
+      <c r="A19" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="15" t="s">
+      <c r="C19" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="G19" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="17" t="s">
+    </row>
+    <row r="20">
+      <c r="A20" s="14" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="15" t="s">
+      <c r="B20" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="17" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" s="14" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="9" t="s">
+      <c r="B21" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="D21" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="E21" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="F21" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="G21" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="9" t="s">
+    </row>
+    <row r="22">
+      <c r="A22" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="B22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="9" t="s">
+      <c r="D22" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="E22" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="F22" s="12"/>
+      <c r="G22" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="17" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="23">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
     </row>
     <row r="24">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
     </row>
     <row r="25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
     </row>
     <row r="26">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
     </row>
     <row r="27">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
     </row>
     <row r="28">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
     </row>
     <row r="29">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="31">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added final submission documentation and asset list.
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
   <si>
     <t>Event Name</t>
   </si>
@@ -346,6 +346,9 @@
     <t>Whirring machinery sound</t>
   </si>
   <si>
+    <t>Modified to include a "wind up" period at start of sound.</t>
+  </si>
+  <si>
     <t>https://freesound.org/people/reklamacja/sounds/446157/</t>
   </si>
   <si>
@@ -489,6 +492,9 @@
   </si>
   <si>
     <t>Several synths, drums</t>
+  </si>
+  <si>
+    <t>Modified to include beeping when player is at low health.</t>
   </si>
   <si>
     <r>
@@ -1226,14 +1232,16 @@
       <c r="E16" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="G16" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>8</v>
@@ -1242,21 +1250,21 @@
         <v>65</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>67</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>19</v>
@@ -1265,102 +1273,104 @@
         <v>65</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F22" s="12"/>
+        <v>95</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="G22" s="17" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">

</xml_diff>